<commit_message>
handled both or and combination conditon added stop  conditions
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED\Development_WorkSpaces\eclipse_phantom_workspace\GFATAM\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,8 @@
     <sheet name="Reference" sheetId="2" r:id="rId1"/>
     <sheet name="Messages" sheetId="3" r:id="rId2"/>
     <sheet name="Rules" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Blacklist" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="261">
   <si>
     <t>Type</t>
   </si>
@@ -721,9 +723,6 @@
     <t>Conditions</t>
   </si>
   <si>
-    <t>encounter_datetime</t>
-  </si>
-  <si>
     <t>{entity:Encounter, property:cough, validate:VALUE, value:YES} AND {entity:Encounter, property:appetite, validate:LIST, value:YES,REFUSED,UNKNOWN}</t>
   </si>
   <si>
@@ -749,13 +748,78 @@
   </si>
   <si>
     <t>Dear {user.getFullName}. {patient.getPatientIdentifier} ka GXP Result Positive aa gaya hai. Please patient ka follow-up visit karain.</t>
+  </si>
+  <si>
+    <t>Treatment Initiation Form</t>
+  </si>
+  <si>
+    <t>FUP-REM</t>
+  </si>
+  <si>
+    <t>Fetch Duration</t>
+  </si>
+  <si>
+    <t>Past 2 hours</t>
+  </si>
+  <si>
+    <t>Past 2 months</t>
+  </si>
+  <si>
+    <t>encounterDatetime</t>
+  </si>
+  <si>
+    <t>return visit date</t>
+  </si>
+  <si>
+    <t>PT-AFB-POS</t>
+  </si>
+  <si>
+    <t>{patient.getFullName}, jitni jaldi ho sakay {patient.getHealthCentre} pe Doctor ke pass moainay ki liyay tashreef laain. Appointment laynay kay liyay 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>SS-AFB-POS</t>
+  </si>
+  <si>
+    <t>Dear {user.getFullName}, PID {patient.getPatientIdentifier} ka {encounter.encounterDate} tareek ko SMEAR Result Positive ({encounter.observations[concept=smear_result}].value), {encounter.encounterLocation} pe aa gaya hai. Please patient ka follow-up visit karain.</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>{entity:Encounter, property:treatment_initiated, validate:VALUE, value:"YES"} 
+AND {entity:Encounter, property:return_visit_date, validate:REGEX, value:""} 
+AND {entity:Patient, property:primaryContact, validate:REGEX, value:"[0-9]+"}</t>
+  </si>
+  <si>
+    <t>return_visit_date</t>
+  </si>
+  <si>
+    <t>CHTB-REM</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>{entity:Encounter, Encounter: End Follow-up, validate:Encounter, after: "Childhood TB-Treatment Initiation"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{entity:Encounter, property:smear_result, validate:LIST, value:" Scanty 3 - 24,THREE PLUS,ONE PLUS ,TWO PLUS"} </t>
+  </si>
+  <si>
+    <t>{entity:Encounter, encounter: End of Followup, validate:Encounter, after: "Childhood TB-Treatment Initiation"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,16 +835,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -788,17 +883,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1084,7 +1218,7 @@
   <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,45 +2318,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="146.140625" customWidth="1"/>
+    <col min="2" max="2" width="146.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="B2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>228</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2233,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2411,7 @@
     <col min="9" max="9" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2278,84 +2439,101 @@
       <c r="I1" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D2" t="s">
-        <v>225</v>
+      <c r="B2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="E2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" t="s">
-        <v>231</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4" t="s">
-        <v>226</v>
-      </c>
-      <c r="E4" t="s">
-        <v>231</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>235</v>
-      </c>
+      <c r="B3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2367,28 +2545,217 @@
           <x14:formula1>
             <xm:f>Reference!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>A7:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G7:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$C$2:$C$208</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>B7:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D7:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="315" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Reference!$D$2:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Reference!$C$2:$C$208</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Reference!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Select notification type">
+          <x14:formula1>
+            <xm:f>Reference!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding code for day in urdu. commiting sms send line.
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="266">
   <si>
     <t>Type</t>
   </si>
@@ -813,13 +813,53 @@
   </si>
   <si>
     <t>{entity:Encounter, encounter: End of Followup, validate:Encounter, after: "Childhood TB-Treatment Initiation"}</t>
+  </si>
+  <si>
+    <t>CHTB-1REM</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>{entity:Encounter, property:treatment_initiated, validate:VALUE, value:"YES"} 
+AND {entity:Encounter, property:return_visit_date, validate:NOTNULL}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{entity:Encounter, Encounter: Childhood TB-TB Treatment Followup, validate:Encounter, after:"Childhood TB-Treatment Initiation"} </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{entity:Encounter, Encounter: End of Followup, validate:Encounter, after: "Childhood TB-Treatment Initiation"}</t>
+    </r>
+  </si>
+  <si>
+    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter[encounterType=Childhood TB-Treatment Initiation].observations[concept=RETURN VISIT DATE].valueDatetime}, barooz [day of week in urdu], {patient.getHealthCenter} pe doctor ke paas moainey aur adwiyaat hasil karne ke liyey tashreef lana hai. Agar is kay mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,8 +888,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -871,6 +919,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -902,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -911,29 +965,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2318,10 +2380,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,7 +2396,7 @@
       <c r="A1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2363,15 +2425,15 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>249</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -2379,11 +2441,19 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2394,9 +2464,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2411,7 +2481,7 @@
     <col min="9" max="9" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2443,97 +2513,37 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="E2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="7">
+      <c r="E2" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" s="9">
         <v>-1</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-    </row>
-    <row r="3" spans="1:26" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="F3" s="10">
-        <v>-1</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
+      <c r="H2" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>262</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2545,25 +2555,25 @@
           <x14:formula1>
             <xm:f>Reference!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A7:A1048576</xm:sqref>
+          <xm:sqref>A5:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G7:G1048576</xm:sqref>
+          <xm:sqref>G5:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$C$2:$C$208</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B1048576</xm:sqref>
+          <xm:sqref>B5:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D7:D1048576</xm:sqref>
+          <xm:sqref>D5:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2573,121 +2583,216 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="10"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="10">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="315" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="10">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="10" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="195" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="10">
         <v>-1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="10" t="s">
         <v>244</v>
       </c>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F29" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F30" s="17">
+        <v>-1</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the Warehouse database connection added Day in Urdu
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED\Development_WorkSpaces\eclipse_phantom_workspace\GFATAM\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="6195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="2" r:id="rId1"/>
@@ -18,7 +13,8 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
     <sheet name="Blacklist" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="E1:L13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="268">
   <si>
     <t>Type</t>
   </si>
@@ -854,11 +850,17 @@
   <si>
     <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter[encounterType=Childhood TB-Treatment Initiation].observations[concept=RETURN VISIT DATE].valueDatetime}, barooz [day of week in urdu], {patient.getHealthCenter} pe doctor ke paas moainey aur adwiyaat hasil karne ke liyey tashreef lana hai. Agar is kay mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
   </si>
+  <si>
+    <t>Fetch Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPENMRS </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -929,7 +931,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -952,11 +954,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -997,6 +1010,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1074,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1092,7 +1109,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1269,7 +1286,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2382,7 +2399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2464,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2479,9 +2496,11 @@
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2512,8 +2531,11 @@
       <c r="J1" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="19" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -2544,8 +2566,16 @@
       <c r="J2" s="7" t="s">
         <v>262</v>
       </c>
+      <c r="K2" s="18" t="s">
+        <v>267</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+      <formula1>"OPENMRS ,DATAWAREHOUSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
setting location name when calling patient.getHealthCenter,
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED\Development_WorkSpaces\team_lead\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="6195" activeTab="2"/>
   </bookViews>
@@ -14,7 +19,6 @@
     <sheet name="Blacklist" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="E1:L13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="268">
   <si>
     <t>Type</t>
   </si>
@@ -743,9 +747,6 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Dear {user.getFullName}. {patient.getPatientIdentifier} ka GXP Result Positive aa gaya hai. Please patient ka follow-up visit karain.</t>
-  </si>
-  <si>
     <t>Treatment Initiation Form</t>
   </si>
   <si>
@@ -770,13 +771,7 @@
     <t>PT-AFB-POS</t>
   </si>
   <si>
-    <t>{patient.getFullName}, jitni jaldi ho sakay {patient.getHealthCentre} pe Doctor ke pass moainay ki liyay tashreef laain. Appointment laynay kay liyay 080011982 pe rabta karain.</t>
-  </si>
-  <si>
     <t>SS-AFB-POS</t>
-  </si>
-  <si>
-    <t>Dear {user.getFullName}, PID {patient.getPatientIdentifier} ka {encounter.encounterDate} tareek ko SMEAR Result Positive ({encounter.observations[concept=smear_result}].value), {encounter.encounterLocation} pe aa gaya hai. Please patient ka follow-up visit karain.</t>
   </si>
   <si>
     <t>User</t>
@@ -814,53 +809,37 @@
     <t>CHTB-1REM</t>
   </si>
   <si>
-    <t>3 months</t>
-  </si>
-  <si>
-    <t>{entity:Encounter, property:treatment_initiated, validate:VALUE, value:"YES"} 
-AND {entity:Encounter, property:return_visit_date, validate:NOTNULL}</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{entity:Encounter, Encounter: Childhood TB-TB Treatment Followup, validate:Encounter, after:"Childhood TB-Treatment Initiation"} </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-{entity:Encounter, Encounter: End of Followup, validate:Encounter, after: "Childhood TB-Treatment Initiation"}</t>
-    </r>
-  </si>
-  <si>
-    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter[encounterType=Childhood TB-Treatment Initiation].observations[concept=RETURN VISIT DATE].valueDatetime}, barooz [day of week in urdu], {patient.getHealthCenter} pe doctor ke paas moainey aur adwiyaat hasil karne ke liyey tashreef lana hai. Agar is kay mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
-  </si>
-  <si>
     <t>Fetch Source</t>
   </si>
   <si>
-    <t xml:space="preserve">OPENMRS </t>
+    <t>Dear {user.getFullName}, {patient.getPatientIdentifier} ka GXP Result Positive aa gaya hai. Please patient ka follow-up visit karain.</t>
+  </si>
+  <si>
+    <t>2 months</t>
+  </si>
+  <si>
+    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.return_visit_date}, barooz [day_of_week_in_urdu], {patient.getHealthCenter} pe doctor ke paas moainey aur adwiyaat hasil karne ke liyey tashreef lana hai. Agar is kay mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>Dear {user.getFullName}, PID {patient.getPatientIdentifier} ka {encounter.encounterDate} tareek ko SMEAR Result Positive ({encounter.smear_result}), {encounter.encounterLocation} pe aa gaya hai. Please patient ka follow-up visit karain.</t>
+  </si>
+  <si>
+    <t>{patient.getFullName}, jitni jaldi ho sakay {patient.getHealthCenter} pe Doctor ke pass moainay ki liyay tashreef laain. Appointment laynay kay liyay 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"treatment_initiated","validate":"VALUE","value":"YES"}AND{"entity":"Encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","Encounter":"Childhood TB-TB Treatment Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}OR{"entity":"Encounter","Encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"Encounter","Encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657}OR{"entity":"Encounter","Encounter":"Referral and Transfer","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"Encounter","Encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER"}</t>
+  </si>
+  <si>
+    <t>OPENMRS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -899,7 +878,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,8 +909,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -954,22 +939,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -981,20 +955,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1010,10 +975,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,7 +1049,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1109,7 +1084,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1286,7 +1261,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2409,68 +2384,64 @@
     <col min="2" max="2" width="146.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>239</v>
+      <c r="B4" s="4" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>248</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>265</v>
+      <c r="A8" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2483,8 +2454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,81 +2472,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="K1" s="19" t="s">
+      <c r="J1" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="F2" s="9">
-        <v>-1</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="18" t="s">
         <v>261</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>262</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>267</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
-      <formula1>"OPENMRS ,DATAWAREHOUSE"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -2585,25 +2551,25 @@
           <x14:formula1>
             <xm:f>Reference!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A5:A1048576</xm:sqref>
+          <xm:sqref>A20:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G5:G1048576</xm:sqref>
+          <xm:sqref>G20:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$C$2:$C$208</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B1048576</xm:sqref>
+          <xm:sqref>B20:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D1048576</xm:sqref>
+          <xm:sqref>D20:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2621,208 +2587,208 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="10">
+      <c r="E1" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="7">
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="10">
-        <v>1</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F4" s="10">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="C29" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="F29" s="14">
+      <c r="E29" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="F29" s="11">
         <v>-1</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
+      <c r="H29" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="C30" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F30" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="F30" s="17">
-        <v>-1</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2877,16 +2843,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ton of changes. Read with care - Extracted Abstract class from SMS Notification Job classes - Changed the columns in ExcelSheetWriter and CsvFileWriter - Added "Record only" column to Excel file to be able to log the messages without sending - Minor bug fixes (while making changes) in Rule entity - Refactored Message entity. Removed some redundant columns and simplified the model - Removed consent variable from Patient entity - Simplified the way dbUtil is set in NotificationJob classes. Reading from the RuleBook - Added method to validate Patient IDs in ValidationUtil - Added Relationship entity to model package - Created SearchService in common project to search for Contacts. INCOMPLETE, UNTESTED
Context:
- Added loadRelationshipTypes() method
- Excluding all patients who have NOT consented while loading patients
- Added getRelationshipsByPersonId() to get all relationships
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED\Development_WorkSpaces\team_lead\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="272">
   <si>
     <t>Type</t>
   </si>
@@ -840,6 +840,12 @@
   </si>
   <si>
     <t>{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-TB Treatment Followup"}AND{"entity":"Encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"}OR{"entity":"Encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"Encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER"}</t>
+  </si>
+  <si>
+    <t>Record Only</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -2475,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2490,11 +2496,11 @@
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="10" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -2528,8 +2534,11 @@
       <c r="K1" s="17" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="17" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
@@ -2563,8 +2572,11 @@
       <c r="K2" s="18" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
@@ -2576,6 +2588,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Changed the sources to fetch metadata to OpenMRS (should change back to DW if it makes more sense) - Added more columns to ExcelSheetWriter class for Rule and Snapshot dates - Constructor added in Rule class - ValidationUtil complete. validateSingleCondition() method also handles the stop conditions - ValidationUtilTest complete - Bug fixed in SmsNotificationsJob. Validation was called twice
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="325">
   <si>
     <t>Type</t>
   </si>
@@ -879,19 +879,7 @@
     <t>TREATMENT COORDINATOR</t>
   </si>
   <si>
-    <t>{"entity":"encounter","property":"treatment_initiated","validate":"VALUE","value":"YES"}AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
-  </si>
-  <si>
     <t>{"entity":"encounter","property":"treatment_plan","validate":"LIST","value":"164439,1257"}AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-TB Treatment Followup"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","property":"reason_for_call","validate":"VALUE","value":"166097"}AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
   </si>
   <si>
     <t>facility_visit_date</t>
@@ -901,52 +889,19 @@
 {"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-Verbal Screening"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
   </si>
   <si>
-    <t>{"entity":"encounter","property":"reason_for_call","validate":"VALUE","value":"165819"}
-AND{"entity":"encounter","property":"reason_for_call","validate":"VALUE","value":165818=NULL}
-AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
-  </si>
-  <si>
     <t>{"entity":"encounter","encounter":"FAST-Treatment Initiation","validate":"encounter","after":"FAST-Presumptive Information"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"FAST-Presumptive Information"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","property":"reason_for_call","validate":"VALUE","value":"165818"}
-AND{"entity":"encounter","property":"reason_for_call","validate":"VALUE","value":"165819"}
-AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
   </si>
   <si>
     <t>{"entity":"encounter","encounter":"GXP Specimen Collection","validate":"encounter","after":"CXR Screening Test Result"}OR{"entity":"encounter","encounter":"GeneXpert Result","validate":"encounter","after":"FAST-Presumptive Information"}AND{"entity":"encounter","encounter":"GeneXpert Result","property":"mtb_result","validate":"LIST","value":"1301,1302"}OR{"entity":"encounter","encounter":"FAST-Treatment Initiation","validate":"encounter","after":"CXR Screening Test Result"}OR
 {"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"CXR Screening Test Result"}</t>
   </si>
   <si>
-    <t>{"entity":"encounter","property":"reason_for_call","validate":"LIST","value":165818}
-AND{"entity":"encounter","property":"reason_for_call","validate":"VALUE","value":165819=NULL}
-AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
-  </si>
-  <si>
     <t>{"entity":"encounter","encounter":"GXP Specimen Collection","validate":"encounter","after":"CC - TB Investigation FUP"}OR{"entity":"encounter","encounter":"GeneXpert Result","validate":"encounter","after":"FAST-Presumptive Information"}AND{"entity":"encounter","encounter":"GeneXpert Result","property":mtb_result,"validate":"LIST","value":1301,1302}OR{"entity":"encounter","encounter":"FAST-Treatment Initiation","validate":"encounter","after":"FAST-Presumptive Information"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"FAST-Presumptive Information"}</t>
   </si>
   <si>
-    <t>{"entity":"encounter","property":"antibiotic","validate":"VALUE","value":"YES"}
-AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","encounter":"FAST-Treatment Initiation","property":"treatment_initiated","validate":"VALUE","value":"YES"}OR
-({"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"FAST-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"})OR({"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"FAST-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER" })</t>
-  </si>
-  <si>
     <t>{"entity":"encounter","property":referral_site,"validate":"NOTNULL"}</t>
   </si>
   <si>
-    <t>{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","property":"treatment_initiated","validate":"VALUE","value":"YES"}
-AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"VALUE","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
-  </si>
-  <si>
     <t>{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
   </si>
   <si>
@@ -954,10 +909,6 @@
   </si>
   <si>
     <t>{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"PET-Treatment Initiation"}OR{"entity":"encounter","encounter":"PET-Refusal Form","validate":"encounter","after":"PET-Treatment Initiation"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","property":"reason_for_home_visit","validate":"VALUE","value":"165854"}
-AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
   </si>
   <si>
     <t>{"entity":"encounter","encounter":PET-"Clinician Evaluation","validate":"encounter","after":"PET-Home Visit"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"PET-Home Visit"}OR{"entity":"encounter","encounter":"PET-Refusal Form","property":"encounterDatetime","validate":"NOTNULL"}</t>
@@ -1036,9 +987,6 @@
     <t>Validate</t>
   </si>
   <si>
-    <t>VALUE</t>
-  </si>
-  <si>
     <t>NOTEQUALS</t>
   </si>
   <si>
@@ -1060,7 +1008,56 @@
     <t>PRESENT/EXISTS</t>
   </si>
   <si>
-    <t>E.g.</t>
+    <t>EQUALS</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"EQUALS","value":"OTHER"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-TB Treatment Followup"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"EQUALS","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"reason_for_call","validate":"EQUALS","value":"166097"}AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"reason_for_call","validate":"EQUALS","value":"165819"}
+AND{"entity":"encounter","property":"reason_for_call","validate":"EQUALS","value":165818=NULL}
+AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"reason_for_call","validate":"EQUALS","value":"165818"}
+AND{"entity":"encounter","property":"reason_for_call","validate":"EQUALS","value":"165819"}
+AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"reason_for_call","validate":"LIST","value":165818}
+AND{"entity":"encounter","property":"reason_for_call","validate":"EQUALS","value":165819=NULL}
+AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"antibiotic","validate":"EQUALS","value":"YES"}
+AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","encounter":"FAST-Treatment Initiation","property":"treatment_initiated","validate":"EQUALS","value":"YES"}OR
+({"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"FAST-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"})OR({"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"FAST-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"EQUALS","value":"OTHER" })</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"treatment_initiated","validate":"EQUALS","value":"YES"}
+AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":"159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657"}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"EQUALS","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"reason_for_home_visit","validate":"EQUALS","value":"165854"}
+AND{"entity":"encounter","property":"facility_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","property":"treatment_initiated","validate":"EQUALS","value":"YES"}AND{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"EQUALS","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1156,6 +1153,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1439,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,17 +1473,15 @@
         <v>280</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>325</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1505,10 +1503,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1531,10 +1529,10 @@
         <v>241</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1555,10 +1553,10 @@
         <v>242</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1573,7 +1571,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1587,7 +1585,7 @@
       </c>
       <c r="E6" s="5"/>
       <c r="H6" s="14" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1599,7 +1597,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="H7" s="14" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1611,7 +1609,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="H8" s="14" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1623,7 +1621,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="H9" s="14" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3577,7 +3575,7 @@
         <v>270</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3641,7 +3639,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,7 +3705,7 @@
         <v>203</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>226</v>
@@ -3725,7 +3723,7 @@
         <v>270</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10" t="s">
@@ -3759,7 +3757,7 @@
         <v>277</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>249</v>
@@ -3847,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,7 +3912,7 @@
         <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>224</v>
@@ -3932,7 +3930,7 @@
         <v>246</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>284</v>
+        <v>324</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>249</v>
@@ -3952,7 +3950,7 @@
         <v>83</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>224</v>
@@ -3970,7 +3968,7 @@
         <v>244</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>249</v>
@@ -3990,13 +3988,13 @@
         <v>150</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>287</v>
+        <v>314</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F4" s="10">
         <v>-1</v>
@@ -4008,7 +4006,7 @@
         <v>258</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10" t="s">
@@ -4025,14 +4023,14 @@
       <c r="B5" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>290</v>
+      <c r="C5" s="17" t="s">
+        <v>315</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F5" s="10">
         <v>-1</v>
@@ -4044,7 +4042,7 @@
         <v>261</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10" t="s">
@@ -4061,14 +4059,14 @@
       <c r="B6" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>292</v>
+      <c r="C6" s="17" t="s">
+        <v>316</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F6" s="10">
         <v>-1</v>
@@ -4080,7 +4078,7 @@
         <v>263</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10" t="s">
@@ -4097,14 +4095,14 @@
       <c r="B7" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>294</v>
+      <c r="C7" s="17" t="s">
+        <v>317</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F7" s="10">
         <v>-1</v>
@@ -4116,7 +4114,7 @@
         <v>265</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10" t="s">
@@ -4133,8 +4131,8 @@
       <c r="B8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>296</v>
+      <c r="C8" s="17" t="s">
+        <v>318</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>224</v>
@@ -4151,8 +4149,8 @@
       <c r="H8" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>297</v>
+      <c r="I8" s="17" t="s">
+        <v>319</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -4167,8 +4165,8 @@
       <c r="B9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>300</v>
+      <c r="C9" s="17" t="s">
+        <v>320</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>224</v>
@@ -4186,7 +4184,7 @@
         <v>271</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>249</v>
@@ -4206,7 +4204,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>224</v>
@@ -4224,7 +4222,7 @@
         <v>273</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>249</v>
@@ -4244,7 +4242,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>224</v>
@@ -4262,7 +4260,7 @@
         <v>274</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>249</v>
@@ -4281,14 +4279,14 @@
       <c r="B12" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>305</v>
+      <c r="C12" s="17" t="s">
+        <v>322</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F12" s="10">
         <v>-1</v>
@@ -4300,7 +4298,7 @@
         <v>275</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>249</v>
@@ -4320,7 +4318,7 @@
         <v>209</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>224</v>
@@ -4338,7 +4336,7 @@
         <v>276</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="J13" s="10" t="s">
         <v>249</v>
@@ -4358,7 +4356,7 @@
         <v>186</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>282</v>
@@ -4376,7 +4374,7 @@
         <v>278</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>249</v>
@@ -4396,7 +4394,7 @@
         <v>186</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>224</v>
@@ -4414,7 +4412,7 @@
         <v>279</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
- Added Treatment Coordinator to the list in getContactFromRule() method in AbstractSmsNotificationsJob - Exception replaced in getReferenceDate() method in Context - More corrections and clean-up in RuleBook
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="323">
   <si>
     <t>Type</t>
   </si>
@@ -705,13 +705,7 @@
     <t>PATIENT</t>
   </si>
   <si>
-    <t>FACILITY</t>
-  </si>
-  <si>
     <t>SUPERVISOR</t>
-  </si>
-  <si>
-    <t>DOCTOR</t>
   </si>
   <si>
     <t>CLINIC-EVAL</t>
@@ -897,9 +891,6 @@
   </si>
   <si>
     <t>{"entity":"encounter","encounter":"GXP Specimen Collection","validate":"encounter","after":"CC - TB Investigation FUP"}OR{"entity":"encounter","encounter":"GeneXpert Result","validate":"encounter","after":"FAST-Presumptive Information"}AND{"entity":"encounter","encounter":"GeneXpert Result","property":mtb_result,"validate":"LIST","value":1301,1302}OR{"entity":"encounter","encounter":"FAST-Treatment Initiation","validate":"encounter","after":"FAST-Presumptive Information"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"FAST-Presumptive Information"}</t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","property":referral_site,"validate":"NOTNULL"}</t>
   </si>
   <si>
     <t>{"entity":"encounter","property":"return_visit_date","validate":"NOTNULL"}</t>
@@ -1002,12 +993,6 @@
     <t>LIST</t>
   </si>
   <si>
-    <t>NOTNULL</t>
-  </si>
-  <si>
-    <t>PRESENT/EXISTS</t>
-  </si>
-  <si>
     <t>EQUALS</t>
   </si>
   <si>
@@ -1058,6 +1043,15 @@
   </si>
   <si>
     <t>{"entity":"encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}OR{"entity":"encounter","encounter":"End of Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"End of Followup","property":"treatment_outcome","validate":"LIST","value":159791,160035,159874,160034,160031,165836,165837,164791,164792,166221,127750,166222,165891,160037,166288,165657}OR{"entity":"encounter","encounter":"Referral and Transfer","validate":"encounter","after":"Childhood TB-Treatment Initiation"}AND{"entity":"encounter","encounter":"Referral and Transfer","property":"referral_site","validate":"EQUALS","value":"OTHER"}OR{"entity":"patient","property":"getHealthCenterId","validate":"query","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>FACILITY/LOCATION</t>
+  </si>
+  <si>
+    <t>NOTNULL/PRESENT/EXISTS</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"referral_site","validate":"NOTNULL"}</t>
   </si>
 </sst>
 </file>
@@ -1440,7 +1434,7 @@
   <dimension ref="A1:I208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1446,7 @@
     <col min="5" max="5" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="71.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1470,16 +1464,16 @@
         <v>223</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I1" s="13"/>
     </row>
@@ -1497,16 +1491,16 @@
         <v>224</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1520,19 +1514,19 @@
         <v>211</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>225</v>
+        <v>320</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G3" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1546,17 +1540,17 @@
         <v>140</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>302</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1566,12 +1560,12 @@
         <v>147</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1580,12 +1574,9 @@
       <c r="C6" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>282</v>
-      </c>
       <c r="E6" s="5"/>
       <c r="H6" s="14" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1597,7 +1588,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="H7" s="14" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,7 +1600,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="H8" s="14" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1620,9 +1611,7 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="H9" s="14" t="s">
-        <v>310</v>
-      </c>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -3442,189 +3431,189 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B22" s="14"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B23" s="14"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B24" s="14"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B25" s="14"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B26" s="14"/>
     </row>
@@ -3636,10 +3625,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3667,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -3685,16 +3674,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3705,13 +3694,13 @@
         <v>203</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>289</v>
+        <v>322</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
@@ -3720,17 +3709,17 @@
         <v>14</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3742,10 +3731,10 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
@@ -3754,20 +3743,19 @@
         <v>14</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>249</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
       <c r="K3" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>252</v>
-      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I5" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3809,9 +3797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3823,16 +3809,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3845,9 +3831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3874,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -3892,16 +3876,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3912,13 +3896,13 @@
         <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F2" s="12">
         <v>-1</v>
@@ -3927,19 +3911,19 @@
         <v>15</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3950,13 +3934,13 @@
         <v>83</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F3" s="12">
         <v>-1</v>
@@ -3965,19 +3949,19 @@
         <v>15</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3988,13 +3972,13 @@
         <v>150</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F4" s="10">
         <v>-1</v>
@@ -4003,20 +3987,20 @@
         <v>15</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -4024,13 +4008,13 @@
         <v>150</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F5" s="10">
         <v>-1</v>
@@ -4039,20 +4023,20 @@
         <v>15</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -4060,13 +4044,13 @@
         <v>150</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F6" s="10">
         <v>-1</v>
@@ -4075,20 +4059,20 @@
         <v>15</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
@@ -4096,13 +4080,13 @@
         <v>150</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F7" s="10">
         <v>-1</v>
@@ -4111,20 +4095,20 @@
         <v>15</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -4132,13 +4116,13 @@
         <v>44</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F8" s="10">
         <v>-1</v>
@@ -4147,18 +4131,18 @@
         <v>15</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
@@ -4166,13 +4150,13 @@
         <v>82</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F9" s="10">
         <v>3</v>
@@ -4181,19 +4165,19 @@
         <v>15</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4204,13 +4188,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F10" s="10">
         <v>-1</v>
@@ -4219,19 +4203,19 @@
         <v>15</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -4242,13 +4226,13 @@
         <v>25</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F11" s="10">
         <v>-1</v>
@@ -4257,22 +4241,22 @@
         <v>15</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
@@ -4280,13 +4264,13 @@
         <v>174</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F12" s="10">
         <v>-1</v>
@@ -4295,19 +4279,19 @@
         <v>15</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4318,13 +4302,13 @@
         <v>209</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F13" s="10">
         <v>-1</v>
@@ -4333,19 +4317,19 @@
         <v>15</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4356,13 +4340,13 @@
         <v>186</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F14" s="10">
         <v>3</v>
@@ -4371,19 +4355,19 @@
         <v>16</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4394,13 +4378,13 @@
         <v>186</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>224</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F15" s="10">
         <v>3</v>
@@ -4409,19 +4393,19 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>281</v>
-      </c>
       <c r="L15" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4430,12 +4414,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Reference!$D$2:$D$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>D18:D1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$C$2:$C$208</xm:f>
@@ -4454,6 +4432,12 @@
           </x14:formula1>
           <xm:sqref>A18:A1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Reference!$D$2:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D18:D1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Big change: * Added validation for the rules in RuleBook when reading - Change in getContactFromRule() in Abstract... user added and treatment coordinator/supporter removed - Bug fixed in parseFormattedMessage() when checking instance of Encounter in Message parser - Bug fixed in searchContactFromEntityValuePair() where space was clipping the last part - More corrections in RuleBook - Removed getScheduleDateTime() from Rule class - Refactored searchValueFromEncounter() method - Made getEntityPropertyValue() more generic by removing restriction of BaseEntity instance checking - Made the exception more detailed when contact is null (only in Sms - Lots of null checks added overall - Some test data manipulation for testing
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18390" windowHeight="6105" tabRatio="740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18390" windowHeight="6105" tabRatio="692" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="314">
   <si>
     <t>Type</t>
   </si>
@@ -994,12 +994,6 @@
     </r>
   </si>
   <si>
-    <t>{"entity":"Encounter","property":mtb_result,"validate":"VALUE","value":"1301"}</t>
-  </si>
-  <si>
-    <t>{"entity":"Encounter","property":mtb_result,"validate":"LIST","value":"1301,1302"}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{"entity":"Encounter","encounter":"FAST-Presumptive","property":"screening_type","validate":"VALUE","value":"165854"}OR
 {"entity":"Encounter","encounter":"FAST-Treatment Initiation","validate":"PRESENT"}
 </t>
@@ -1026,6 +1020,15 @@
   </si>
   <si>
     <t>Dear {user.getFullName}, PID {patient.getPatientIdentifier} {location.getLocationName} pe register ho gay hain. In say rabta karain.</t>
+  </si>
+  <si>
+    <t>Search Relationship.TREATMENT COORDINATOR</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"mtb_result","validate":"VALUE","value":"1301"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"mtb_result","validate":"LIST","value":"1301,1302"}</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1565,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="H7" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3394,7 +3397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3426,7 +3429,7 @@
         <v>250</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3434,7 +3437,7 @@
         <v>255</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3442,7 +3445,7 @@
         <v>300</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3450,7 +3453,7 @@
         <v>301</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3467,8 +3470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,7 +3537,7 @@
         <v>203</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>225</v>
@@ -3569,7 +3572,7 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>231</v>
@@ -3600,7 +3603,7 @@
         <v>187</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>224</v>
@@ -3618,7 +3621,7 @@
         <v>300</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10" t="s">
@@ -3636,7 +3639,7 @@
         <v>187</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>224</v>
@@ -3654,7 +3657,7 @@
         <v>301</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10" t="s">

</xml_diff>

<commit_message>
- Made ReminderSmsNotificationJob class consistent with SmsNotificationJob - Added NotificationType column to Excel writer - Creating log file in a separate directory - Output directory now reading from properties file - Helpline number corrected on excel sheet
</commit_message>
<xml_diff>
--- a/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
+++ b/gfatm-notifications-sms/src/main/resources/rules/RuleBook.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SADEEQA\Desktop\automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\gfatm-notifications\gfatm-notifications-sms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6300" tabRatio="692" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6300" tabRatio="692" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="335">
   <si>
     <t>Type</t>
   </si>
@@ -1000,15 +1000,6 @@
     <t>{"entity":"Encounter","property":"referral_site","validate":"NOTEQUALS","value":"OTHER"}</t>
   </si>
   <si>
-    <t>Dear {patient.getFullName}, ap ko {patient.getHealthCentre} pe doctor ke paas {encounter.return_visit_date} ko moainey aur adwiyaat hasil karne ke liyey tashreef lana tha mager aap na aa sakay. Bara-e-Meherbani, apnay muainay kay liyay tashreef laiyay. Ager aap apna muqarrara muaina kerwa chukay hain, to is SMS ko nazar andaaz kejiyay. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 0800-11982 pe rabta karain.</t>
-  </si>
-  <si>
-    <t>Dear {patient.getFullName}, {patient.getPatientIdentifierLocation} pe ap nay balgham ka namoona jama kiya tha jis ka result aa gaya hai. Bara-e-mehrbani aap aa kar apna result wusool kar lain. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 021-111-111-982 pe rabta karain.</t>
-  </si>
-  <si>
-    <t>Dear {patient.getFullName}, {patient.getPatientIdentifierLocation} pe ap nay balgham ka namoona jama kiya tha jiska result aa gaya hai. Bara-e-Mehrbani aap aa kar apna result wusool kar lain. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 021-111-111-982 pe rabta karain.</t>
-  </si>
-  <si>
     <t>Dear {user.getFullName}, PID {patient.getPatientIdentifier} {location.getLocationName} pe register ho gay hain. In say rabta karain.</t>
   </si>
   <si>
@@ -1016,27 +1007,10 @@
   </si>
   <si>
     <t>{"entity":"Encounter","property":"gxp_result","validate":"LIST","value":"1301,1302"}</t>
-  </si>
-  <si>
-    <t>{"entity":"Encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}
-OR{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-TB Treatment Followup"}</t>
-  </si>
-  <si>
-    <t>-- DONT SEND IF
-select distinct pt.patient_id from patient as pt 
--- Chtb Tx Initiation
-inner join encounter as pres on pres.encounter_type = 210 and pres.patient_id = pt.patient_id and pres.voided = 0 
--- Chtb Tx fup exists after initiaion
-where exists (select * from encounter as e where e.voided = 0 and e.encounter_type = 68 and e.patient_id = pt.patient_id and e.encounter_datetime &gt; pres.encounter_datetime);</t>
   </si>
   <si>
     <t xml:space="preserve">{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-TB Treatment Followup"}
 </t>
-  </si>
-  <si>
-    <t>{"entity":"encounter","Encounter":"Childhood TB-TB Treatment Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}
-OR{"entity":"encounter","Encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}
-OR{"entity":"encounter","encounter":"Missed Visit Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}</t>
   </si>
   <si>
     <t>-- DONT SEND IF
@@ -1051,13 +1025,6 @@
   </si>
   <si>
     <t>CC-CHTB-TEST-REM</t>
-  </si>
-  <si>
-    <t>{"entity":"Encounter","encounter":Childhood TB-Antibiotic Trial Initiation,"validate":"Encounter","after":"Clinician Evaluation"}
-OR{"entity":"Encounter","encounter":PET-Infection Treatment Eligibility,"validate":"Encounter","after":"Clinician Evaluation"}
-OR{"entity":"Encounter","encounter":Childhood TB-Treatment Initiation,"validate":"Encounter","after":"Clinician Evaluation"}
-OR{"entity":"Encounter","encounter":PET-Treatment Initiation,"validate":"Encounter","after":"Clinician Evaluation"}
-OR{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Clinician Evaluation"}</t>
   </si>
   <si>
     <t>-- DONT SEND IF
@@ -1080,10 +1047,6 @@
     <t>CC-CHTB-MO-EVAL</t>
   </si>
   <si>
-    <t>{"entity":"Encounter","encounter":"Clinician Evaluation","validate":"Encounter","after":"Childhood TB-Verbal Screening"}
-OR{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-Verbal Screening"}</t>
-  </si>
-  <si>
     <t>-- DONT SEND IF
 select distinct pt.patient_id from patient as pt 
 -- Chtb Verbal Screening
@@ -1098,38 +1061,95 @@
     <t>{"entity":"Encounter","property":"gxp_result","validate":"EQUALS","value":"1301"}</t>
   </si>
   <si>
-    <t>{"entity":"Encounter","property":"treatment_plan","validate":"LIST","value":"164439,1257"}AND{"entity":"Encounter","property":"return_visit_date","validate":"NOTNULL"}AND{"entity":"patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
-  </si>
-  <si>
-    <t>{"entity":"Encounter","property":"reason_for_call","validate":"EQUALS","value":"165816"}AND{"entity":"Encounter","property":"facility_visit_date","validate":"NOTNULL"}AND{"entity":"patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
-  </si>
-  <si>
-    <t>{"entity":"Encounter","property":"reason_for_call","validate":"EQUALS","value":"166097"}AND{"entity":"Encounter","property":"facility_visit_date","validate":"NOTNULL"}AND{"entity":"patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
-  </si>
-  <si>
-    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.return_visit_date}, barooz {encounter.return_visit_date.day}, {patient.getHealthCentre} pe doctor ke paas moainey aur adwiyaat hasil karne ke liyey tashreef lana hai. Agar is kay mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
-  </si>
-  <si>
-    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.facility_visit_date}, barooz {encounter.facility_visit_date.day}, {encounter.facility_scheduled} pe doctor ke paas moainey ke liyey tashreef lana hai. Agar Ap pechle 3 din me tashreef la chuke he to iss message ko nazar andaz kar de. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
-  </si>
-  <si>
-    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.facility_visit_date}, barooz {encounter.return_visit_date.day}, {encounter.facility_scheduled} pe test result lay ke doctor ke paas moainey ke liyey tashreef lana hai. Agar Ap pechle 3 din me tashreef la chuke he to iss message ko nazar andaz kar de. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
-  </si>
-  <si>
-    <t>{patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.facility_visit_date}, barooz {encounter.return_visit_date.day}, {encounter.facility_scheduled} pe doctor ke paas moainey ke liyey tashreef lana hai. Agar Ap pechle 3 din me tashreef la chuke he to iss message ko nazar andaz kar de. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"entity":"Encounter","encounter":"FAST-Presumptive","property":"screening_type","validate":"EQUALS","value":"165988"}OR
-{"entity":"Encounter","encounter":"FAST-Treatment Initiation","validate":"PRESENT"}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"entity":"Encounter","encounter":"FAST-Presumptive","property":"screening_type","validate":"EQUALS","value":"165854"}OR
-{"entity":"Encounter","encounter":"FAST-Treatment Initiation","validate":"PRESENT"}
-</t>
-  </si>
-  <si>
-    <t>{"entity":"Encounter","property":"treatment_initiated","validate":"EQUALS","value":"1065"}AND{"entity":"Encounter","property":"return_visit_date","validate":"NOTNULL"}AND{"entity":"patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+    <t>Dear {patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.facility_visit_date}, baroz {encounter.facility_visit_date.day}, {encounter.facility_scheduled} pe doctor ke paas moainey ke liyey tashreef lana hai. Agar Ap pechle 3 din me tashreef la chuke he to iss message ko nazar andaz kar de. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>Dear {patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.facility_visit_date}, baroz {encounter.return_visit_date.day}, {encounter.facility_scheduled} pe test result lay ke doctor ke paas moainey ke liyey tashreef lana hai. Agar Ap pechle 3 din me tashreef la chuke he to iss message ko nazar andaz kar de. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>Dear {patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.facility_visit_date}, baroz {encounter.return_visit_date.day}, {encounter.facility_scheduled} pe doctor ke paas moainey ke liyey tashreef lana hai. Agar Ap pechle 3 din me tashreef la chuke he to iss message ko nazar andaz kar de. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>Dear {patient.getFullName}, aap ko yaad karana chahtain hain kay ap ko {encounter.return_visit_date}, baroz {encounter.return_visit_date.day}, AaoTBMitao ki facility {patient.getHealthCentre} pe doctor ke paas moainey aur adwiyaat hasil karne ke liyey tashreef lana hai. Agar is kay mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","encounter":"FAST-Presumptive","property":"screening_type","validate":"EQUALS","value":"165988"}OR
+{"entity":"Encounter","encounter":"FAST-Treatment Initiation","validate":"PRESENT"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","encounter":"FAST-Presumptive","property":"screening_type","validate":"EQUALS","value":"165854"}OR
+{"entity":"Encounter","encounter":"FAST-Treatment Initiation","validate":"PRESENT"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"treatment_initiated","validate":"EQUALS","value":"1065"}
+AND
+{"entity":"Encounter","property":"return_visit_date","validate":"NOTNULL"}
+AND
+{"entity":"Patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"treatment_plan","validate":"LIST","value":"164439,1257"}
+AND
+{"entity":"Encounter","property":"return_visit_date","validate":"NOTNULL"}
+AND
+{"entity":"Patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"reason_for_call","validate":"EQUALS","value":"165816"}
+AND
+{"entity":"Encounter","property":"facility_visit_date","validate":"NOTNULL"}
+AND
+{"entity":"Patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","property":"reason_for_call","validate":"EQUALS","value":"166097"}
+AND
+{"entity":"Encounter","property":"facility_visit_date","validate":"NOTNULL"}
+AND
+{"entity":"Patient","property":"getHealthCenterId","validate":"QUERY","value":"SELECT location_id FROM location WHERE name not in ( 'SGHNK-KHI','IHK-KHI','GHAURI-CLINIC','ICD-KTR');"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","encounter":"Childhood TB-TB Treatment Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}
+OR
+{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-TB Treatment Followup"}</t>
+  </si>
+  <si>
+    <t>{"entity":"encounter","Encounter":"Childhood TB-TB Treatment Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}
+OR
+{"entity":"encounter","Encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-Treatment Initiation"}
+OR
+{"entity":"encounter","encounter":"Missed Visit Followup","validate":"encounter","after":"Childhood TB-Treatment Initiation"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","encounter":Childhood TB-Antibiotic Trial Initiation,"validate":"Encounter","after":"Clinician Evaluation"}
+OR
+{"entity":"Encounter","encounter":PET-Infection Treatment Eligibility,"validate":"Encounter","after":"Clinician Evaluation"}
+OR
+{"entity":"Encounter","encounter":Childhood TB-Treatment Initiation,"validate":"Encounter","after":"Clinician Evaluation"}
+OR
+{"entity":"Encounter","encounter":PET-Treatment Initiation,"validate":"Encounter","after":"Clinician Evaluation"}
+OR
+{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Clinician Evaluation"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Encounter","encounter":"Clinician Evaluation","validate":"Encounter","after":"Childhood TB-Verbal Screening"}
+OR
+{"entity":"Encounter","encounter":"End of Followup","validate":"Encounter","after":"Childhood TB-Verbal Screening"}</t>
+  </si>
+  <si>
+    <t>{"entity":"Patient","property":"getPatientId","validate":"QUERY","value":"select distinct pt.patient_id from patient as pt inner join encounter as pres on pres.encounter_type = 210 and pres.patient_id = pt.patient_id and pres.voided = 0 where exists (select * from encounter as e where e.voided = 0 and e.encounter_type = 68 and e.patient_id = pt.patient_id and e.encounter_datetime &gt; pres.encounter_datetime);"}"</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Dear {patient.getFullName}, ap ko {patient.getHealthCentre} pe doctor ke paas {encounter.return_visit_date} ko moainey aur adwiyaat hasil karne ke liyey tashreef lana tha mager aap na aa sakay. Bara-e-Meherbani, apnay muainay kay liyay tashreef laiyay. Ager aap apna muqarrara muaina kerwa chukay hain, to is SMS ko nazar andaaz kejiyay. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>Dear {patient.getFullName}, AaoTBMitao ki facility {patient.getPatientIdentifierLocation} pe ap nay balgham ka namoona jama kiya tha jis ka result aa gaya hai. Bara-e-mehrbani aap aa kar apna result wusool kar lain. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
+  </si>
+  <si>
+    <t>Dear {patient.getFullName}, {patient.getPatientIdentifierLocation} pe ap nay balgham ka namoona jama kiya tha jiska result aa gaya hai. Bara-e-Mehrbani aap aa kar apna result wusool kar lain. Agar is mutaliq ap kuch poochna chahain tou AaoTBMitao helpline 080011982 pe rabta karain.</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1220,14 +1240,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1511,8 +1537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,9 +1664,7 @@
       <c r="C5" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>260</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="14"/>
       <c r="H5" s="14" t="s">
@@ -1932,7 +1957,7 @@
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -3507,103 +3532,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="157.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="157.140625" style="17" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>308</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>306</v>
+      <c r="B5" s="16" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="B6" s="16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="16" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>327</v>
+      <c r="B8" s="16" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>328</v>
+      <c r="B9" s="20" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>329</v>
+      <c r="A10" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>330</v>
+      <c r="A11" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3616,15 +3642,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="14"/>
     <col min="2" max="2" width="32" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="171.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
@@ -3634,45 +3661,49 @@
     <col min="10" max="10" width="14.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="14"/>
+    <col min="13" max="13" width="73.85546875" style="14" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="18" t="s">
         <v>242</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3708,6 +3739,7 @@
       <c r="L2" s="10" t="s">
         <v>243</v>
       </c>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -3718,7 +3750,7 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>231</v>
@@ -3740,8 +3772,9 @@
       <c r="L3" s="10" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -3749,7 +3782,7 @@
         <v>187</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>224</v>
@@ -3766,8 +3799,8 @@
       <c r="H4" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>331</v>
+      <c r="I4" s="16" t="s">
+        <v>320</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10" t="s">
@@ -3776,8 +3809,9 @@
       <c r="L4" s="10" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -3785,7 +3819,7 @@
         <v>187</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>224</v>
@@ -3802,8 +3836,8 @@
       <c r="H5" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>332</v>
+      <c r="I5" s="16" t="s">
+        <v>321</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10" t="s">
@@ -3812,207 +3846,209 @@
       <c r="L5" s="10" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="C6" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="16">
         <v>-1</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="16">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8" s="16">
+        <v>3</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="300" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="16">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F10" s="16">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="I10" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="J10" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K10" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L10" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="M6" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F7" s="10">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F8" s="10">
-        <v>3</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="F9" s="10">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="F10" s="10">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>320</v>
+      <c r="M10" s="16" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4030,7 +4066,7 @@
           <x14:formula1>
             <xm:f>Reference!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G12:G13 G14:G1048576</xm:sqref>
+          <xm:sqref>G12:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4042,13 +4078,13 @@
           <x14:formula1>
             <xm:f>Reference!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D6 D12:D13 D14:D1048576</xm:sqref>
+          <xm:sqref>D6 D12:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Select notification type">
           <x14:formula1>
             <xm:f>Reference!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A6:A10 A12:A13 A14:A1048576</xm:sqref>
+          <xm:sqref>A6:A10 A12:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4094,7 +4130,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>